<commit_message>
New script for LTP in range
</commit_message>
<xml_diff>
--- a/csv_files/merged_data_without_LTP.xlsx
+++ b/csv_files/merged_data_without_LTP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imadc\PycharmProjects\fwdproject\csv_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA6DF54-A0F9-4BF2-A5A9-53E6186D2A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7F190F-6806-4745-8210-0DC229D6AA90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BA25306F-F9BE-412F-841E-D4614913F7ED}"/>
   </bookViews>
@@ -397,7 +397,7 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>